<commit_message>
Updated Dates and assignee
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>S.No</t>
   </si>
@@ -316,6 +316,21 @@
 Promotions :=&gt; 1.) Buy one get one free.
                                 2.) Get SD card free with Samsung mobiles.
 </t>
+  </si>
+  <si>
+    <t>Swapnil</t>
+  </si>
+  <si>
+    <t>Swarnima</t>
+  </si>
+  <si>
+    <t>Swarnima / Swapnil</t>
+  </si>
+  <si>
+    <t>Create Addon named "healthpromotionsaddon"</t>
+  </si>
+  <si>
+    <t>Create a separate functionality altogether. Including bncwebservices</t>
   </si>
 </sst>
 </file>
@@ -445,22 +460,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -511,6 +520,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,430 +828,565 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="16" customWidth="1"/>
     <col min="5" max="6" width="11.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="73.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+    <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>42012</v>
+      </c>
+      <c r="F2" s="6">
+        <v>42012</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C3" s="15">
         <v>0.5</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D3" s="15">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="10" t="s">
+      <c r="E3" s="6">
+        <v>42012</v>
+      </c>
+      <c r="F3" s="6">
+        <v>42012</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="15">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6">
+        <v>42012</v>
+      </c>
+      <c r="F4" s="6">
+        <v>42012</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C5" s="15">
         <v>3</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D5" s="15">
         <v>24</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="10" t="s">
+      <c r="E5" s="6">
+        <v>42013</v>
+      </c>
+      <c r="F5" s="6">
+        <v>42017</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>3</v>
-      </c>
-      <c r="B4" s="14" t="s">
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="15">
+        <v>4</v>
+      </c>
+      <c r="E6" s="6">
+        <v>42012</v>
+      </c>
+      <c r="F6" s="6">
+        <v>42012</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="15">
         <v>12</v>
       </c>
-      <c r="C4" s="17">
+      <c r="E7" s="6">
+        <v>42012</v>
+      </c>
+      <c r="F7" s="6">
+        <v>42013</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="15">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6">
+        <v>42023</v>
+      </c>
+      <c r="F8" s="6">
+        <v>42023</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="15">
         <v>0.5</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D9" s="15">
         <v>4</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="10" t="s">
+      <c r="E9" s="6">
+        <v>42018</v>
+      </c>
+      <c r="F9" s="6">
+        <v>42018</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="15">
+        <v>4</v>
+      </c>
+      <c r="E10" s="6">
+        <v>42018</v>
+      </c>
+      <c r="F10" s="6">
+        <v>42018</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>9</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="15">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6">
+        <v>42019</v>
+      </c>
+      <c r="F11" s="6">
+        <v>42019</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="D12" s="15">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6">
+        <v>42019</v>
+      </c>
+      <c r="F12" s="6">
+        <v>42023</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15">
+        <v>8</v>
+      </c>
+      <c r="E13" s="6">
+        <v>42024</v>
+      </c>
+      <c r="F13" s="6">
+        <v>42024</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="D14" s="15">
+        <v>20</v>
+      </c>
+      <c r="E14" s="6">
+        <v>42025</v>
+      </c>
+      <c r="F14" s="6">
+        <v>42027</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <v>13</v>
       </c>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="B15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="15">
+        <v>20</v>
+      </c>
+      <c r="E15" s="6">
+        <v>42027</v>
+      </c>
+      <c r="F15" s="6">
+        <v>42032</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
+      <c r="D16" s="15">
+        <v>16</v>
+      </c>
+      <c r="E16" s="6">
+        <v>42033</v>
+      </c>
+      <c r="F16" s="6">
+        <v>42034</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>15</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="17">
+      <c r="E17" s="6">
+        <v>42025</v>
+      </c>
+      <c r="F17" s="6">
+        <v>42025</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>16</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="15">
         <v>0.5</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D18" s="15">
         <v>4</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14" t="s">
+      <c r="E18" s="6">
+        <v>42025</v>
+      </c>
+      <c r="F18" s="6">
+        <v>42025</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>17</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2</v>
+      </c>
+      <c r="D19" s="15">
         <v>16</v>
       </c>
-      <c r="C6" s="17">
+      <c r="E19" s="6">
+        <v>42026</v>
+      </c>
+      <c r="F19" s="6">
+        <v>42027</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23">
+        <v>18</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="19">
         <v>1.5</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D20" s="19">
         <v>12</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>6</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="17">
-        <v>1</v>
-      </c>
-      <c r="D7" s="17">
-        <v>8</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>7</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="17">
-        <v>4</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <v>8</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="17">
-        <v>4</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>9</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="17">
-        <v>4</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="17">
-        <v>2.5</v>
-      </c>
-      <c r="D11" s="17">
-        <v>20</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>11</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="17">
-        <v>1</v>
-      </c>
-      <c r="D12" s="17">
-        <v>8</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>12</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="17">
-        <v>2.5</v>
-      </c>
-      <c r="D13" s="17">
-        <v>20</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <v>13</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="17">
-        <v>2.5</v>
-      </c>
-      <c r="D14" s="17">
-        <v>20</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <v>14</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="17">
-        <v>2</v>
-      </c>
-      <c r="D15" s="17">
-        <v>16</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
-        <v>15</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="D16" s="17">
-        <v>4</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="D17" s="17">
-        <v>4</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
-        <v>17</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="17">
-        <v>2</v>
-      </c>
-      <c r="D18" s="17">
-        <v>16</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <v>18</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="21">
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="21">
-        <v>12</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="23" t="s">
+      <c r="E20" s="6">
+        <v>42031</v>
+      </c>
+      <c r="F20" s="6">
+        <v>42032</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="13"/>
+      <c r="I20" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Revert "Updates tasks""
This reverts commit 774fca9337141ed87ae1fb55af63529de13b883a.
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -90,8 +90,196 @@
     <t xml:space="preserve">After above steps &amp; hybris update verify that new products have been added in database and are accessible on PDP pages etc. </t>
   </si>
   <si>
-    <t>Create a new data model for managing health related customer data.
-Note: It should extend User Data model.</t>
+    <t>Create web service to get all the customer exercise data (heartbeat, blood pressure, miles, calories, time, age) through url of the web service.</t>
+  </si>
+  <si>
+    <t>Implementation of backend logic to save all the data retrieved from web service in database.</t>
+  </si>
+  <si>
+    <t>This will involve façade, service, dao layer etc.</t>
+  </si>
+  <si>
+    <t>Create promotional web service specific to beacon id.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is customer specific promotion so beaconId need not be present here.
+The idea is to group the target customers based on there health data and then offer promotions to them.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> All the customers who run more than 1 Mile per day can be offered discount on sports shoes.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create few promotions and assign a relevant user group (having your target customer) to it.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Create Impex for the same.</t>
+    </r>
+  </si>
+  <si>
+    <t>Create one more promotional web service specific to the customer.
+This will return all the promotions that are applicable for the user group of this user.</t>
+  </si>
+  <si>
+    <t>This URL of the web service will be like :
+http://localhost:9001/bncwebservices/v1/electronics/CustomerHealthPromotions/neeraj.a.shah@accenture.com
+Here the only parameter "neeraj.a.shah@accenture" is the unique email id of the user.
+Note: This webservice will return all the promotions associated with the mention user.</t>
+  </si>
+  <si>
+    <t>Create a cron job to send mails to the customers who are eligible for promotions.</t>
+  </si>
+  <si>
+    <t>This will involve new entry in item.xml, spring.xml, extension of job performable class and implementation of perform method() having logic to retrieve all the customers that are eligible for promotions.
+Note: It will internally use above mention web service to check for the promotions based on customer Id.</t>
+  </si>
+  <si>
+    <t>Triggering emails to the customer.</t>
+  </si>
+  <si>
+    <t>This will involve setting up SMTP server , setting up mail templates and then triggering mail to the customer with the relevant promotion information retrieved from the above web service.</t>
+  </si>
+  <si>
+    <t>Extend the Product data model to add "beaconId" and "location" attributes.</t>
+  </si>
+  <si>
+    <t>This is done to associate products with beacon id and to store location of the products . (location will be seprated by ‘|’ character e.g. Aisle 2B|Wing 4|Floor 3)</t>
+  </si>
+  <si>
+    <t>Create Impex to insert beaconId and location data in the product table.</t>
+  </si>
+  <si>
+    <t>This data will be used by relevant web services.</t>
+  </si>
+  <si>
+    <t>Create web service to retrieve all the product details (location etc) depending on the beacon id.</t>
+  </si>
+  <si>
+    <t>Customize OOB product based web service to return beacon Id and location details of the product along with other OOB product details.</t>
+  </si>
+  <si>
+    <t>Effort (hours)</t>
+  </si>
+  <si>
+    <t>Create a new item type "beacon" having following attributes:
+1.) Id
+2.) MajorId
+3.) MinorId
+4.) Welcome Message</t>
+  </si>
+  <si>
+    <t>This will hold data for all beacon including its major &amp; minor Id.</t>
+  </si>
+  <si>
+    <t>Create a N-N relation between "beacon" and "AbstractPromotions"</t>
+  </si>
+  <si>
+    <t>This relation is required because multiple promotions can be associated with one beacon and at same time one promotion can be associated with multiple beacon also, hence N-N relation.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create few promotions and beacon instances through HMC and associate the promotions with beacon instances so created.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Create Impex for the same.</t>
+    </r>
+  </si>
+  <si>
+    <t>This is to be done through HMC.
+The idea is to have multiple instances of promotions and beacon present in the database so that the promotional webservice could retrieve the same.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This URL of the web service will be like :
+http://localhost:9001/bncwebservices/v1/electronics/BeaconPromotions/eda4b92b-07ab-4ca4-8ecd-43d53123bd98/000001/000002
+Here "eda4b92b-07ab-4ca4-8ecd-43d53123bd98" is beacon id, "000001" is major Id and "000002" is minor Id.
+Note: This webservice will return the welcome message and all the promotions associated with this beacon id.
+Example : Welcome Message :=&gt; Welcome to our Store! 30 % off on Digital cameras for today only.
+Promotions :=&gt; 1.) Buy one get one free.
+                                2.) Get SD card free with Samsung mobiles.
+</t>
+  </si>
+  <si>
+    <t>Swapnil</t>
+  </si>
+  <si>
+    <t>Swarnima</t>
+  </si>
+  <si>
+    <t>Swarnima / Swapnil</t>
+  </si>
+  <si>
+    <t>Create Addon named "healthpromotionsaddon"</t>
+  </si>
+  <si>
+    <t>Create a separate functionality altogether. Including bncwebservices</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Swapnil</t>
+  </si>
+  <si>
+    <t>Create a new data model for managing health related customer data.</t>
   </si>
   <si>
     <t>This new data model "CustomerHealthData" should have following fields:
@@ -100,18 +288,22 @@
 (3) Miles run
 (4) Calories burned
 (5) Time taken
-(6) Age</t>
-  </si>
-  <si>
-    <t>Create web service to get all the customer exercise data (heartbeat, blood pressure, miles, calories, time, age) through url of the web service.</t>
-  </si>
-  <si>
-    <t>Implementation of backend logic to save all the data retrieved from web service in database.</t>
+(6) Age
+(7) CustomerId</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">The web service will be accessible through following URL.
-http://localhost:9001/bncwebservices/v1/electronics/CustomerHealthData/60/100/1.5/150/30/29
+http://localhost:9001/bncwebservices/v1/electronics/CustomerHealthData
+The values shall be passed as a JSON object as follows:
+{‘HealthData’:
+ [
+  {‘type’: ‘customerId’, ‘Value’ : ‘123’},
+  {‘type’: ‘heartbeatrate’, ‘Value’ : ‘72’},
+  {‘type’: ‘bloodPressure’, ‘Value’ : ‘80’}
+ ]
+}
+and so on..
 </t>
     </r>
     <r>
@@ -144,107 +336,8 @@
     </r>
   </si>
   <si>
-    <t>This will involve façade, service, dao layer etc.</t>
-  </si>
-  <si>
-    <t>Create promotional web service specific to beacon id.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is customer specific promotion so beaconId need not be present here.
-The idea is to group the target customers based on there health data and then offer promotions to them.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Example:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> All the customers who run more than 1 Mile per day can be offered discount on sports shoes.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create few promotions and assign a relevant user group (having your target customer) to it.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Create Impex for the same.</t>
-    </r>
-  </si>
-  <si>
-    <t>Create one more promotional web service specific to the customer.
-This will return all the promotions that are applicable for the user group of this user.</t>
-  </si>
-  <si>
-    <t>This URL of the web service will be like :
-http://localhost:9001/bncwebservices/v1/electronics/CustomerHealthPromotions/neeraj.a.shah@accenture.com
-Here the only parameter "neeraj.a.shah@accenture" is the unique email id of the user.
-Note: This webservice will return all the promotions associated with the mention user.</t>
-  </si>
-  <si>
-    <t>Create a cron job to send mails to the customers who are eligible for promotions.</t>
-  </si>
-  <si>
-    <t>This will involve new entry in item.xml, spring.xml, extension of job performable class and implementation of perform method() having logic to retrieve all the customers that are eligible for promotions.
-Note: It will internally use above mention web service to check for the promotions based on customer Id.</t>
-  </si>
-  <si>
-    <t>Triggering emails to the customer.</t>
-  </si>
-  <si>
-    <t>This will involve setting up SMTP server , setting up mail templates and then triggering mail to the customer with the relevant promotion information retrieved from the above web service.</t>
-  </si>
-  <si>
-    <t>Extend the Product data model to add "beaconId" and "location" attributes.</t>
-  </si>
-  <si>
-    <t>This is done to associate products with beacon id and to store location of the products . (location will be seprated by ‘|’ character e.g. Aisle 2B|Wing 4|Floor 3)</t>
-  </si>
-  <si>
-    <t>Create Impex to insert beaconId and location data in the product table.</t>
-  </si>
-  <si>
-    <t>This data will be used by relevant web services.</t>
-  </si>
-  <si>
-    <t>Create web service to retrieve all the product details (location etc) depending on the beacon id.</t>
-  </si>
-  <si>
     <t xml:space="preserve">This URL of the web service will be like :_x000D_
-http://localhost:9001/bncwebservices/v1/electronics/ProductsLocationDetails/eda4b92b-07ab-4ca4-8ecd-43d53123bd98/_x000D_
+http://localhost:9001/bncwebservices/v1/electronics/ProductLocationDetails/eda4b92b-07ab-4ca4-8ecd-43d53123bd98/_x000D_
 _x000D_
 Here the only parameter "eda4b92b-07ab-4ca4-8ecd-43d53123bd98" is beacon id._x000D_
 _x000D_
@@ -252,91 +345,7 @@
 </t>
   </si>
   <si>
-    <t>Customize OOB product based web service to return beacon Id and location details of the product along with other OOB product details.</t>
-  </si>
-  <si>
-    <t>This will require customization of OOB product webservice (http://localhost:9001/bncwebservice/v1/electronics/products/553637?options=DESCRIPTION) to return product location &amp; beacon Id associate with that product.</t>
-  </si>
-  <si>
-    <t>Effort (hours)</t>
-  </si>
-  <si>
-    <t>Create a new item type "beacon" having following attributes:
-1.) Id
-2.) MajorId
-3.) MinorId
-4.) Welcome Message</t>
-  </si>
-  <si>
-    <t>This will hold data for all beacon including its major &amp; minor Id.</t>
-  </si>
-  <si>
-    <t>Create a N-N relation between "beacon" and "AbstractPromotions"</t>
-  </si>
-  <si>
-    <t>This relation is required because multiple promotions can be associated with one beacon and at same time one promotion can be associated with multiple beacon also, hence N-N relation.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create few promotions and beacon instances through HMC and associate the promotions with beacon instances so created.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Create Impex for the same.</t>
-    </r>
-  </si>
-  <si>
-    <t>This is to be done through HMC.
-The idea is to have multiple instances of promotions and beacon present in the database so that the promotional webservice could retrieve the same.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This URL of the web service will be like :
-http://localhost:9001/bncwebservices/v1/electronics/BeaconPromotions/eda4b92b-07ab-4ca4-8ecd-43d53123bd98/000001/000002
-Here "eda4b92b-07ab-4ca4-8ecd-43d53123bd98" is beacon id, "000001" is major Id and "000002" is minor Id.
-Note: This webservice will return the welcome message and all the promotions associated with this beacon id.
-Example : Welcome Message :=&gt; Welcome to our Store! 30 % off on Digital cameras for today only.
-Promotions :=&gt; 1.) Buy one get one free.
-                                2.) Get SD card free with Samsung mobiles.
-</t>
-  </si>
-  <si>
-    <t>Swapnil</t>
-  </si>
-  <si>
-    <t>Swarnima</t>
-  </si>
-  <si>
-    <t>Swarnima / Swapnil</t>
-  </si>
-  <si>
-    <t>Create Addon named "healthpromotionsaddon"</t>
-  </si>
-  <si>
-    <t>Create a separate functionality altogether. Including bncwebservices</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Swapnil</t>
+    <t>This will require customization of OOB product webservice (http://localhost:9001/bncwebservices/v1/electronics/products/553637?options=DESCRIPTION) to return product location &amp; beacon Id associate with that product.</t>
   </si>
 </sst>
 </file>
@@ -831,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +867,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>6</v>
@@ -881,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C2" s="13">
         <v>0</v>
@@ -896,13 +905,13 @@
         <v>42012</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -925,13 +934,13 @@
         <v>42012</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -954,13 +963,13 @@
         <v>42012</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -983,21 +992,21 @@
         <v>42026</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C6" s="13">
         <v>0.5</v>
@@ -1012,21 +1021,21 @@
         <v>42012</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="335.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="13">
         <v>1.5</v>
@@ -1041,13 +1050,13 @@
         <v>42013</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1055,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="13">
         <v>1</v>
@@ -1070,13 +1079,13 @@
         <v>42023</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1084,7 +1093,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C9" s="13">
         <v>0.5</v>
@@ -1099,13 +1108,13 @@
         <v>42025</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1113,7 +1122,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C10" s="13">
         <v>0.5</v>
@@ -1128,13 +1137,13 @@
         <v>42025</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1142,7 +1151,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C11" s="13">
         <v>0.5</v>
@@ -1157,13 +1166,13 @@
         <v>42026</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1171,7 +1180,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="13">
         <v>2.5</v>
@@ -1186,13 +1195,13 @@
         <v>42031</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1200,7 +1209,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="13">
         <v>1</v>
@@ -1215,13 +1224,13 @@
         <v>42027</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="173.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1229,7 +1238,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="13">
         <v>2.5</v>
@@ -1244,13 +1253,13 @@
         <v>42032</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1258,7 +1267,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C15" s="13">
         <v>2.5</v>
@@ -1273,13 +1282,13 @@
         <v>42033</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1287,7 +1296,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C16" s="13">
         <v>2</v>
@@ -1302,13 +1311,13 @@
         <v>42037</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1316,7 +1325,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C17" s="13">
         <v>0.5</v>
@@ -1331,13 +1340,13 @@
         <v>42033</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1345,7 +1354,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" s="13">
         <v>0.5</v>
@@ -1360,13 +1369,13 @@
         <v>42033</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -1374,7 +1383,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
@@ -1389,13 +1398,13 @@
         <v>42037</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1403,7 +1412,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C20" s="17">
         <v>1.5</v>
@@ -1418,13 +1427,13 @@
         <v>42039</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added defects and additional tasks
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Defects" sheetId="3" r:id="rId2"/>
+    <sheet name="Addtnl Tasks" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
   <si>
     <t>S.No</t>
   </si>
@@ -346,6 +347,79 @@
   </si>
   <si>
     <t>This will require customization of OOB product webservice (http://localhost:9001/bncwebservices/v1/electronics/products/553637?options=DESCRIPTION) to return product location &amp; beacon Id associate with that product.</t>
+  </si>
+  <si>
+    <t>Defect description</t>
+  </si>
+  <si>
+    <t>OOB products and category pages not opening - 404 not found error</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Send UCOID along with the other order details through in existing webservice</t>
+  </si>
+  <si>
+    <t>Change the return type of Beacon webservice to JSON</t>
+  </si>
+  <si>
+    <t>Customer Health Data webservice not recognising the customer. Showing customer not found.</t>
+  </si>
+  <si>
+    <t>Products are not adding to recently viewed list when viewed from the mobile application</t>
+  </si>
+  <si>
+    <t>Existing UI fixes:</t>
+  </si>
+  <si>
+    <t>Remove dependency on bncstorefront for dummy images for customers showing on csr dashboard</t>
+  </si>
+  <si>
+    <t>Image size fix for left navigation</t>
+  </si>
+  <si>
+    <t>Change the bell shound for both Customers and Orders Dashboard</t>
+  </si>
+  <si>
+    <t>Carousel functionality for wishlist, recently viewed and recommended products not working.</t>
+  </si>
+  <si>
+    <t>Align customer details properly on personal page on orders dashboard</t>
+  </si>
+  <si>
+    <t>% sign not showing in target</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Create a new webservice for detecting a beacon and performing 2 tasks - showing promotions and welcome messages, and adding customer to the waiting queue
+Merge the 2 existing webservices for beacon detection in 1</t>
+  </si>
+  <si>
+    <t>Integration of new UI</t>
+  </si>
+  <si>
+    <t>Swarnima/Swapnil</t>
+  </si>
+  <si>
+    <t>Currently On Hold</t>
+  </si>
+  <si>
+    <t>Change the return type of Customer Health Data webservice to JSON</t>
+  </si>
+  <si>
+    <t>Create a new webservice for retrieving all the beacon ids and their major and minor ids</t>
+  </si>
+  <si>
+    <t>Create a new webservice for retrieving all the customer's collect orders</t>
+  </si>
+  <si>
+    <t>Add the additional Customer Health Data attributes and modify related code for the saving the health data for the customer</t>
+  </si>
+  <si>
+    <t>Move the default beacon and their major and minor ids to properties file(the beacon which adds the customer to the waiting queue) for easy change in future</t>
   </si>
 </sst>
 </file>
@@ -391,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -471,11 +545,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,6 +632,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -1444,12 +1564,464 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="30"/>
+    <col min="2" max="2" width="85.7109375" style="30" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="30"/>
+    <col min="6" max="6" width="14.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>6</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>8</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>9</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22">
+        <v>10</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22">
+        <v>11</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28">
+        <v>12</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="30"/>
+    <col min="2" max="2" width="85.7109375" style="30" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="30"/>
+    <col min="6" max="6" width="23.42578125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>6</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>8</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>9</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22">
+        <v>10</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22">
+        <v>11</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28">
+        <v>12</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="27"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the tasks for 2-3-4 March wishlist handling
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="84">
   <si>
     <t>S.No</t>
   </si>
@@ -420,6 +420,39 @@
   </si>
   <si>
     <t>Move the default beacon and their major and minor ids to properties file(the beacon which adds the customer to the waiting queue) for easy change in future</t>
+  </si>
+  <si>
+    <t>Create webservice for sending all wishlist products for the customer.</t>
+  </si>
+  <si>
+    <t>This webservice will receive the JSON object as {customerId:"1234"}
+And it will send the List&lt;Product&gt; 
+The URL of the webservice will be:
+http://localhost:9001/bncwebservices/v1/electronics/wishlist/get</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Create webservice for adding a product to the wishlist for a customer</t>
+  </si>
+  <si>
+    <t>This webservice will receive the JSON object as {customerId:"1234",productId:"4567"}
+And it will send the List&lt;Product&gt; 
+The URL of the webservice will be:
+http://localhost:9001/bncwebservices/v1/electronics/wishlist/add</t>
+  </si>
+  <si>
+    <t>Create webservice for removing a product from the wishlist for a customer</t>
+  </si>
+  <si>
+    <t>This webservice will receive the JSON object as {customerId:"1234",productId:"4567"}
+And it will send the List&lt;Product&gt; 
+The URL of the webservice will be:
+http://localhost:9001/bncwebservices/v1/electronics/wishlist/remove</t>
+  </si>
+  <si>
+    <t>Explanation</t>
   </si>
 </sst>
 </file>
@@ -465,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -567,11 +600,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -609,9 +688,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -656,6 +732,60 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -958,16 +1088,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="34" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="14" customWidth="1"/>
     <col min="5" max="6" width="11.85546875" style="1" customWidth="1"/>
@@ -980,7 +1110,7 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -1009,7 +1139,7 @@
       <c r="A2" s="13">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="33" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="13">
@@ -1024,13 +1154,13 @@
       <c r="F2" s="6">
         <v>42012</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1059,7 +1189,7 @@
       <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1088,7 +1218,7 @@
       <c r="H4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1111,13 +1241,13 @@
       <c r="F5" s="6">
         <v>42026</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>42</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1146,7 +1276,7 @@
       <c r="H6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1175,7 +1305,7 @@
       <c r="H7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1204,7 +1334,7 @@
       <c r="H8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1233,7 +1363,7 @@
       <c r="H9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1262,7 +1392,7 @@
       <c r="H10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1270,7 +1400,7 @@
       <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="13">
@@ -1291,7 +1421,7 @@
       <c r="H11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1320,7 +1450,7 @@
       <c r="H12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1343,13 +1473,13 @@
       <c r="F13" s="6">
         <v>42027</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1372,13 +1502,13 @@
       <c r="F14" s="6">
         <v>42032</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1407,7 +1537,7 @@
       <c r="H15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1436,7 +1566,7 @@
       <c r="H16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1462,10 +1592,10 @@
       <c r="G17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1491,10 +1621,10 @@
       <c r="G18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1523,21 +1653,21 @@
       <c r="H19" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21">
+      <c r="A20" s="20">
         <v>18</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="16">
         <v>1.5</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>12</v>
       </c>
       <c r="E20" s="6">
@@ -1549,12 +1679,28 @@
       <c r="G20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="22" t="s">
-        <v>45</v>
-      </c>
+      <c r="I20" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="H22" s="31"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="H23" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1572,233 +1718,233 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="30"/>
-    <col min="2" max="2" width="85.7109375" style="30" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="30"/>
-    <col min="6" max="6" width="14.28515625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="30"/>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="2" max="2" width="85.7109375" style="29" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="29"/>
+    <col min="6" max="6" width="14.28515625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28">
+      <c r="A13" s="27">
         <v>12</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="26" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1809,217 +1955,271 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="30"/>
-    <col min="2" max="2" width="85.7109375" style="30" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="30"/>
-    <col min="6" max="6" width="23.42578125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="2" max="2" width="85.7109375" style="29" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="29"/>
+    <col min="6" max="6" width="23.42578125" style="29" customWidth="1"/>
+    <col min="7" max="7" width="70.85546875" style="29" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="G2" s="26"/>
+      <c r="H2" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="B9" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="40">
+        <v>1</v>
+      </c>
+      <c r="D9" s="46">
+        <v>42065</v>
+      </c>
+      <c r="E9" s="41">
+        <v>42065</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="B10" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="42">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>42066</v>
+      </c>
+      <c r="E10" s="43">
+        <v>42066</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="11" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="27"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="B11" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="44">
+        <v>1</v>
+      </c>
+      <c r="D11" s="47">
+        <v>42067</v>
+      </c>
+      <c r="E11" s="45">
+        <v>42067</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27">
         <v>12</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated tasks and status
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="86">
   <si>
     <t>S.No</t>
   </si>
@@ -437,22 +437,28 @@
     <t>Explanation</t>
   </si>
   <si>
-    <t>This webservice will receive the JSON object as {uid:"sdsf@cccccbc.com"}
+    <t>This webservice will receive the JSON object as {"uid":"sdsf@cccccbc.com"}
 And it will send the ProductDataList
 The URL of the webservice will be:
 http://localhost:9001/bncwebservices/v1/electronics/wishlist/get</t>
   </si>
   <si>
-    <t>This webservice will receive the JSON object as {uid:"sdsf@cccccbc.com",productId:"4567"}
+    <t>This webservice will receive the JSON object as {"uid":"sdsf@cccccbc.com","productId":"4567"}
 And it will send the ProductDataList 
 The URL of the webservice will be:
 http://localhost:9001/bncwebservices/v1/electronics/wishlist/add</t>
   </si>
   <si>
-    <t>This webservice will receive the JSON object as {uid:"sdsf@cccccbc.com",productId:"4567"}
+    <t>This webservice will receive the JSON object as {"uid":"sdsf@cccccbc.com","productId":"4567"}
 And it will send the ProductDataList 
 The URL of the webservice will be:
 http://localhost:9001/bncwebservices/v1/electronics/wishlist/remove</t>
+  </si>
+  <si>
+    <t>Modify the beacon promotions webservices, to send out the promotions based on the customer's and beacon's promotions groups</t>
+  </si>
+  <si>
+    <t>Modify the beacon promotions webservices, to send out the promotions based on the customer's and beacon's promotions groups(with no duplications)</t>
   </si>
 </sst>
 </file>
@@ -498,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -624,11 +630,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -747,14 +775,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1927,7 +1967,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,10 +2145,10 @@
       <c r="D9" s="44">
         <v>42065</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="43">
         <v>42066</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="45" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2128,13 +2168,13 @@
       <c r="C10" s="41">
         <v>1</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="46">
         <v>42066</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="6">
         <v>42067</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="26" t="s">
         <v>41</v>
       </c>
       <c r="G10" s="31" t="s">
@@ -2151,16 +2191,16 @@
       <c r="B11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="42">
         <v>1</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="46">
         <v>42066</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="6">
         <v>42067</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="48" t="s">
         <v>40</v>
       </c>
       <c r="G11" s="39" t="s">
@@ -2170,16 +2210,28 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="B12" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="42">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>42067</v>
+      </c>
+      <c r="E12" s="6">
+        <v>42068</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>85</v>
+      </c>
       <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2188,9 +2240,9 @@
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="F13" s="48"/>
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Updated status""
This reverts commit 14cfd7f3a6630ba68488a65358274f83a8bd1389.
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
   <si>
     <t>S.No</t>
   </si>
@@ -423,9 +423,6 @@
   </si>
   <si>
     <t>Create webservice for sending all wishlist products for the customer.</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Create webservice for adding a product to the wishlist for a customer</t>
@@ -2000,7 +1997,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H1" s="24" t="s">
         <v>7</v>
@@ -2152,7 +2149,7 @@
         <v>41</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="37" t="s">
         <v>45</v>
@@ -2163,7 +2160,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="41">
         <v>1</v>
@@ -2178,7 +2175,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H10" s="37" t="s">
         <v>45</v>
@@ -2189,7 +2186,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="42">
         <v>1</v>
@@ -2204,7 +2201,7 @@
         <v>40</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H11" s="37" t="s">
         <v>45</v>
@@ -2215,7 +2212,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="42">
         <v>1</v>
@@ -2230,10 +2227,10 @@
         <v>41</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="26" t="s">
-        <v>77</v>
+        <v>84</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated status and defects
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
   <si>
     <t>S.No</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t xml:space="preserve">Change the beacon item type and make the beaconid, majorId and minorId unique attributes. Also test with the impexes to see whether beacon with same beaconId and different major and minor Ids are being saved to the database. </t>
+  </si>
+  <si>
+    <t>The accordion on order history tab overlaps the order details with other accordion tabs</t>
   </si>
 </sst>
 </file>
@@ -1798,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,8 +2169,8 @@
       <c r="F20" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="51" t="s">
-        <v>66</v>
+      <c r="G20" s="26" t="s">
+        <v>54</v>
       </c>
       <c r="H20" s="51"/>
     </row>
@@ -2184,10 +2187,26 @@
       <c r="F21" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="51" t="s">
+      <c r="G21" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="51"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
+      <c r="B22" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="51"/>
+      <c r="H22" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated defects and additional tasks for use case 2
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="107">
   <si>
     <t>S.No</t>
   </si>
@@ -498,6 +498,37 @@
   </si>
   <si>
     <t>The accordion on order history tab overlaps the order details with other accordion tabs</t>
+  </si>
+  <si>
+    <t>Regarding the promotions notifications showing on IOS App - The welcome message is coming as heading for the promotions. We need to show the welcome messages separately</t>
+  </si>
+  <si>
+    <t>Regarding the promotions notifications showing on IOS App - On click of the promotions, it is redirecting to HAC as the URL at the back end of the promotions is wrong. We need to remove the url on click of the promotions, Instead we can show the alert type pop-up on click of the promotions, which will show the full promotions message with code and validity</t>
+  </si>
+  <si>
+    <t>The promotions are only showing when the customer is logged into the IOS App. Need to fix this as it should show the promotions even when the customer is not logged in, as we will be using the device id to recognise the promotions list.</t>
+  </si>
+  <si>
+    <t>The categories names seems to be hardcoded in the IOS App. It should be dynamic based on the category code</t>
+  </si>
+  <si>
+    <t>The health products category is not showing on the IOS App.</t>
+  </si>
+  <si>
+    <t>Change the orders dashboard UI with the new one.</t>
+  </si>
+  <si>
+    <t>keep the threshold values in local.properties.</t>
+  </si>
+  <si>
+    <t>Change the customerhealthdatawebservice to send out the promotions after saving the customer's health details.
+Take reference from WebserviceFactoryController for sending out the list of promotions.
+While saving the customer's health data, also assign the promotions to the customer based on some conditions.
+The conditions should be as follows:
+Create some sample promotions. Check if the heart rate, or miles run are greater than some value, then assign the related promotions to the customer.</t>
+  </si>
+  <si>
+    <t>IOS App</t>
   </si>
 </sst>
 </file>
@@ -543,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -681,17 +712,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -723,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -797,12 +817,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -833,18 +847,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -857,25 +865,31 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1188,7 +1202,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="32" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="14" customWidth="1"/>
     <col min="5" max="6" width="11.85546875" style="1" customWidth="1"/>
@@ -1230,7 +1244,7 @@
       <c r="A2" s="13">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="31" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="13">
@@ -1778,20 +1792,20 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="H22" s="31"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="H22" s="29"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="H23" s="31"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="H23" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1801,20 +1815,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="85.7109375" style="29" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="29"/>
-    <col min="6" max="6" width="14.28515625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="29"/>
-    <col min="8" max="8" width="67.42578125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="48"/>
+    <col min="2" max="2" width="85.7109375" style="27" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="27"/>
+    <col min="6" max="6" width="14.28515625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="27"/>
+    <col min="8" max="8" width="67.42578125" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1839,7 +1853,7 @@
       <c r="G1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="43" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2027,186 +2041,278 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="50">
+      <c r="A13" s="44">
         <v>12</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51" t="s">
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="51" t="s">
+      <c r="G13" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="51"/>
+      <c r="H13" s="45"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="50">
+      <c r="A14" s="44">
         <v>13</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51" t="s">
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="51" t="s">
+      <c r="H14" s="45" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="50">
+      <c r="A15" s="44">
         <v>14</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51" t="s">
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="51" t="s">
+      <c r="H15" s="45" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="50">
+      <c r="A16" s="44">
         <v>15</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51" t="s">
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="51" t="s">
+      <c r="G16" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="H16" s="51"/>
+      <c r="H16" s="45"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="50">
+      <c r="A17" s="44">
         <v>16</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="51" t="s">
+      <c r="G17" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="51"/>
+      <c r="H17" s="45"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="50">
+      <c r="A18" s="44">
         <v>17</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51" t="s">
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45" t="s">
         <v>41</v>
       </c>
       <c r="G18" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="51"/>
+      <c r="H18" s="45"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
+      <c r="A19" s="46">
         <v>18</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53" t="s">
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="53"/>
+      <c r="H19" s="47"/>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="50">
+      <c r="A20" s="44">
         <v>19</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51" t="s">
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45" t="s">
         <v>41</v>
       </c>
       <c r="G20" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="51"/>
+      <c r="H20" s="45"/>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="50">
+      <c r="A21" s="44">
         <v>20</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51" t="s">
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45" t="s">
         <v>40</v>
       </c>
       <c r="G21" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="51"/>
+      <c r="H21" s="45"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51" t="s">
+      <c r="A22" s="44">
+        <v>21</v>
+      </c>
+      <c r="B22" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51" t="s">
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="51" t="s">
+      <c r="G22" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="51"/>
+      <c r="H22" s="45"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="44">
+        <v>21</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="45"/>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="44">
+        <v>21</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="45"/>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="44">
+        <v>21</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="45"/>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="44">
+        <v>21</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="45"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="44">
+        <v>21</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2215,20 +2321,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="2" max="2" width="85.7109375" style="29" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="29"/>
-    <col min="6" max="6" width="23.42578125" style="29" customWidth="1"/>
-    <col min="7" max="7" width="70.85546875" style="29" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="48"/>
+    <col min="2" max="2" width="85.7109375" style="27" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="27"/>
+    <col min="6" max="6" width="23.42578125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="70.85546875" style="27" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2250,7 +2356,7 @@
       <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="33" t="s">
         <v>79</v>
       </c>
       <c r="H1" s="24" t="s">
@@ -2387,25 +2493,25 @@
       <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="37">
         <v>1.5</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="40">
         <v>42065</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="39">
         <v>42066</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="35" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2416,10 +2522,10 @@
       <c r="B10" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="38">
         <v>1</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="42">
         <v>42066</v>
       </c>
       <c r="E10" s="6">
@@ -2428,76 +2534,110 @@
       <c r="F10" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="38">
         <v>1</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="42">
         <v>42066</v>
       </c>
       <c r="E11" s="6">
         <v>42067</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H11" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
+      <c r="H11" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="44">
         <v>11</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="49">
         <v>1</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="50">
         <v>42067</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="50">
         <v>42068</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
+      <c r="H12" s="45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="44">
         <v>12</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
+      <c r="B13" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="45">
+        <v>2</v>
+      </c>
+      <c r="D13" s="51">
+        <v>42097</v>
+      </c>
+      <c r="E13" s="51">
+        <v>42100</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+    </row>
+    <row r="14" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" s="44">
+        <v>13</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="45">
+        <v>2</v>
+      </c>
+      <c r="D14" s="51">
+        <v>42097</v>
+      </c>
+      <c r="E14" s="51">
+        <v>42100</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated tasks for Use case 3 and defects for Use Case 2
Updated tasks for Use case 3 and defects for Use Case 2
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="109">
   <si>
     <t>S.No</t>
   </si>
@@ -404,9 +404,6 @@
     <t>Swarnima/Swapnil</t>
   </si>
   <si>
-    <t>Currently On Hold</t>
-  </si>
-  <si>
     <t>Change the return type of Customer Health Data webservice to JSON</t>
   </si>
   <si>
@@ -529,6 +526,15 @@
   </si>
   <si>
     <t>IOS App</t>
+  </si>
+  <si>
+    <t>The webservice to send all beacons uuid has been implemented in Hybris. Now this has to be linked in IOS app such that the app should only detect the beacons which have the uuids returned by the webservice.</t>
+  </si>
+  <si>
+    <t>Will wait till the new UI is made responsive</t>
+  </si>
+  <si>
+    <t>On Hold</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,6 +576,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -890,6 +902,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1195,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
@@ -1817,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +1873,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2063,19 +2082,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="45"/>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
       <c r="F14" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="45" t="s">
         <v>66</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2083,19 +2102,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="45"/>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
       <c r="F15" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="45" t="s">
         <v>66</v>
       </c>
       <c r="H15" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2103,13 +2122,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
       <c r="F16" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="45" t="s">
         <v>66</v>
@@ -2121,13 +2140,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
       <c r="F17" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="45" t="s">
         <v>66</v>
@@ -2139,7 +2158,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
@@ -2157,7 +2176,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
@@ -2175,7 +2194,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
@@ -2193,7 +2212,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" s="45"/>
       <c r="D21" s="45"/>
@@ -2211,7 +2230,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22" s="45"/>
       <c r="D22" s="45"/>
@@ -2229,13 +2248,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
       <c r="F23" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>66</v>
@@ -2247,13 +2266,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C24" s="45"/>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>66</v>
@@ -2265,13 +2284,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" s="45"/>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
       <c r="F25" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>66</v>
@@ -2283,13 +2302,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" s="45"/>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
       <c r="F26" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>66</v>
@@ -2301,13 +2320,13 @@
         <v>21</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" s="45"/>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
       <c r="F27" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>66</v>
@@ -2321,10 +2340,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,7 +2376,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" s="24" t="s">
         <v>7</v>
@@ -2396,7 +2415,7 @@
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2404,7 +2423,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
@@ -2422,7 +2441,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
@@ -2440,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -2458,7 +2477,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -2476,7 +2495,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
@@ -2494,7 +2513,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="37">
         <v>1.5</v>
@@ -2509,7 +2528,7 @@
         <v>41</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" s="35" t="s">
         <v>45</v>
@@ -2520,7 +2539,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="38">
         <v>1</v>
@@ -2535,7 +2554,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" s="35" t="s">
         <v>45</v>
@@ -2546,7 +2565,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="38">
         <v>1</v>
@@ -2561,7 +2580,7 @@
         <v>40</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H11" s="35" t="s">
         <v>45</v>
@@ -2572,7 +2591,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="49">
         <v>1</v>
@@ -2587,7 +2606,7 @@
         <v>41</v>
       </c>
       <c r="G12" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" s="45" t="s">
         <v>45</v>
@@ -2598,29 +2617,29 @@
         <v>12</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="45">
         <v>2</v>
       </c>
-      <c r="D13" s="51">
-        <v>42097</v>
-      </c>
-      <c r="E13" s="51">
-        <v>42100</v>
-      </c>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
       <c r="F13" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
+      <c r="G13" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="45" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="44">
         <v>13</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="45">
         <v>2</v>
@@ -2635,9 +2654,25 @@
         <v>40</v>
       </c>
       <c r="G14" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H14" s="45"/>
+    </row>
+    <row r="15" spans="1:8" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="53">
+        <v>14</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new tasks as per UI
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="125">
   <si>
     <t>S.No</t>
   </si>
@@ -542,9 +542,6 @@
 2. condition - String</t>
   </si>
   <si>
-    <t>Create an impex for the above itemtype. With message and condition should be like Rainy, Sunny, Cloudy, Snowy.</t>
-  </si>
-  <si>
     <t>Make related changes for populator and add attributes in existing data object.</t>
   </si>
   <si>
@@ -554,28 +551,92 @@
     <t>In Progress</t>
   </si>
   <si>
-    <t>UI Integration with CSR Dashboard.Dependent on Senthil. After we receive the UI, then we will need to make changes in the CustomersListController as well as JSP. Also in PickInStoreOrdersController for CustomersProfile.</t>
-  </si>
-  <si>
-    <t>Create 2 attributes in Customer Itemtype. Latitudes and Longitudes - type List of Strings</t>
-  </si>
-  <si>
-    <t>Swapnil/Swarnima</t>
-  </si>
-  <si>
-    <t>Based on the above research, create promotions impex with entry for the ranges. Leave out the beacons details in the impex for those promotions</t>
-  </si>
-  <si>
     <t>Add an attribute in the AbstractPromotions itemtype named condition - String type.</t>
   </si>
   <si>
-    <t>Do research and document on ranges for rainy, sunny, cloudy, snowy weather.
+    <t>Create 3 attributes in Customer Itemtype. Latitudes and Longitudes, Date - type List of Strings and List&lt;Date&gt;</t>
+  </si>
+  <si>
+    <t>Create a new webservice which will retrieve the latitude and longitude from the IOS App.
+The URL would be /getGeoLocation
+Method would be POST
+The request body should be in the following format:
+{
+"lat":"12.32",
+"long":"10.23",
+"customerId":"example@email.com"
+}
+Find the customer based on the ID.
+The values should be saved in the Customers Table against the attributes created above. with the condition that if the details already exist in the last entry then not to save the data.</t>
+  </si>
+  <si>
+    <t>Create CustomersGeoData in beans.xml with Data and String as attributes.</t>
+  </si>
+  <si>
+    <r>
+      <t>Inside the same controller method, retrieve the latest entry from List of latitudes and longitudes.
+Using this entry execute the URL for finding out the weather:
+http://api.worldweatheronline.com/free/v2/weather.ashx?q=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45%2C-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;format=json&amp;num_of_days=1&amp;date=today&amp;fx=no&amp;mca=no&amp;fx24=no&amp;includelocation=yes&amp;show_comments=yes&amp;showlocaltime=yes&amp;key=61c3cc6652f35c4e318b62ff3b196
+From the result, we will consider onlyt the following 4 fields:
+1. temperature
+2. Humidity
+3. CloudCover
+4. Precipitation(mm)
+Based on a few conditions, identify the climate as a String
+Add the latitude, longitude and Climate to the model.</t>
+    </r>
+  </si>
+  <si>
+    <t>Inside CustomersListController, create a new ajax method.
+Retrieve the list of lat/long/date from customers table.
+In the loop, execute a webservice which will give the zip, country, state, city with latitude and longitude(in this order) as inputs as follows
+http://api.wunderground.com/auto/wui/geo/GeoLookupXML/index.xml?query=37.76834106,-122.39418793 
+From Output we need to consider only following fields:
+&lt;country&gt;US&lt;/country&gt;
+&lt;state&gt;CA&lt;/state&gt;
+&lt;city&gt;San Francisco&lt;/city&gt;
+&lt;zip&gt;94107&lt;/zip&gt;
+Add these values as San Francisco, 94107 CA, US in a String and save in the CustomersGeoData object along with the date(from the List&lt;Date&gt; for the same index.)
+Add this List&lt;CustomersGeoData&gt; to the model.</t>
+  </si>
+  <si>
+    <t>Create promotions impex with entry for the light rain, moderate rain, heavy rain, sunny, cloudy, light snow, moderate snow, heavy snow weathers. Leave out the beacons details in the impex for those promotions</t>
+  </si>
+  <si>
+    <t>Do research and document on ranges forlight rain, moderate rain, heavy rain, sunny, cloudy, light snow, moderate snow, heavy snow weather.
 After research lets discuss on the ranges needed for identifying the weather clearly. Based on that we will add the properties for min-max range in local.properties.</t>
   </si>
   <si>
+    <t>Create an impex for the above itemtype. With message and condition should be like light rain, moderate rain, heavy rain, sunny, cloudy, light snow, moderate snow, heavy snow.</t>
+  </si>
+  <si>
+    <t>Integrate the HTML of "Geo Location" tab with the existing code as per the code sent by Senthil.
+Create this as a fragment jsp named geoLocations.jsp</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Create a web service which will based on the location data, hit a webservice URL as follows to get the weather information:
-</t>
+      <t>Create a new webservice and combine the code of the above web service which will execute a webservice URL as follows to get the weather information:</t>
     </r>
     <r>
       <rPr>
@@ -639,32 +700,21 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-From the result we receive after hitting the URL, we will retrieve 3 key values from the response:
+From the result we receive after hitting the URL, we will retrieve 4 key values from the response:
 1. temperature
 2. Humidity
 3. CloudCover
-Next this webservice will retrieve the promotions based on the range.
-After that it will check the condition for Rainy, Sunny, Cloudy, Snowy(if else conditions for checking the ranges based on the research) and retrieve the greeting message from the Greeting itemtype based on the condition.
-The final response of the webservice would include:
-1. Greeting
-2. Promotions
-in json format
-The URL would be /greetCustomer
-Method as POST.</t>
+4. Precipitation(mm)
+Next based on some conditions, after identifying the climate, it will retrieve the promotions and greetings based on the climate.
+The final response of the webservice would include(in BeaconPromotionsData):
+1. Greeting as welcome message
+2. Promotions as List of promotionsdata
+URL : /greetCustomer
+POST</t>
     </r>
   </si>
   <si>
-    <t>Create a new webservice which will retrieve the latitude and longitude from the IOS App.
-The URL would be /getGeoLocation
-Method would be POST
-The request body should be in the following format:
-{
-"lat":"12.32",
-"long":"10.23",
-"customerId":"example@email.com"
-}
-Find the customer based on the ID.
-The values should be saved in the Customers Table against the attributes created above.</t>
+    <t>Add the tabs in the main jsp. On click of this particular tab, create an ajax method which will call the above created controller method and retrieve and populate all the data in the jsp.</t>
   </si>
 </sst>
 </file>
@@ -913,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1081,6 +1131,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2510,10 +2567,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2842,10 +2899,10 @@
         <v>40</v>
       </c>
       <c r="G15" s="54" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H15" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2862,7 +2919,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="54" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H16" s="54" t="s">
         <v>45</v>
@@ -2882,13 +2939,13 @@
         <v>40</v>
       </c>
       <c r="G17" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H17" s="54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="55"/>
       <c r="B18" s="56"/>
       <c r="C18" s="54"/>
@@ -2902,9 +2959,11 @@
         <v>40</v>
       </c>
       <c r="G18" s="54" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" s="54"/>
+        <v>119</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="19" spans="1:8" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="55"/>
@@ -2926,7 +2985,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="55"/>
       <c r="B20" s="56"/>
       <c r="C20" s="54"/>
@@ -2940,10 +2999,10 @@
         <v>41</v>
       </c>
       <c r="G20" s="54" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="H20" s="54" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
@@ -2960,7 +3019,7 @@
         <v>41</v>
       </c>
       <c r="G21" s="54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H21" s="54" t="s">
         <v>45</v>
@@ -2980,7 +3039,7 @@
         <v>41</v>
       </c>
       <c r="G22" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H22" s="54" t="s">
         <v>45</v>
@@ -3000,13 +3059,13 @@
         <v>41</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H23" s="54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="52" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="52" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="53">
         <v>14</v>
       </c>
@@ -3024,13 +3083,13 @@
         <v>40</v>
       </c>
       <c r="G24" s="54" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="52" customFormat="1" ht="396" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="52" customFormat="1" ht="355.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="55"/>
       <c r="B25" s="56"/>
       <c r="C25" s="54"/>
@@ -3044,13 +3103,13 @@
         <v>41</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H25" s="54" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="55"/>
       <c r="B26" s="56"/>
       <c r="C26" s="54"/>
@@ -3058,15 +3117,87 @@
         <v>42142</v>
       </c>
       <c r="E26" s="57">
+        <v>42142</v>
+      </c>
+      <c r="F26" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="H26" s="54"/>
+    </row>
+    <row r="27" spans="1:8" s="52" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+      <c r="A27" s="55"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="57">
+        <v>42142</v>
+      </c>
+      <c r="E27" s="57">
         <v>42143</v>
       </c>
-      <c r="F26" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="G26" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="54"/>
+      <c r="F27" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="54"/>
+    </row>
+    <row r="28" spans="1:8" s="52" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="A28" s="55"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="57">
+        <v>42143</v>
+      </c>
+      <c r="E28" s="57">
+        <v>42143</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" s="54"/>
+    </row>
+    <row r="29" spans="1:8" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="55"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="60">
+        <v>42144</v>
+      </c>
+      <c r="E29" s="60">
+        <v>42144</v>
+      </c>
+      <c r="F29" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="59"/>
+    </row>
+    <row r="30" spans="1:8" s="61" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="53"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="57">
+        <v>42144</v>
+      </c>
+      <c r="E30" s="57">
+        <v>42144</v>
+      </c>
+      <c r="F30" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="H30" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated dev plan for IOS tasks
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Defects" sheetId="3" r:id="rId2"/>
     <sheet name="Addtnl Tasks" sheetId="4" r:id="rId3"/>
+    <sheet name="IOS Dev" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="137">
   <si>
     <t>S.No</t>
   </si>
@@ -712,6 +713,54 @@
 Based on a few conditions, as used in the above webservice, identify the climate as a String
 Add the latitude, longitude and Climate to the model.</t>
     </r>
+  </si>
+  <si>
+    <t>Set up the Hybris</t>
+  </si>
+  <si>
+    <t>Mayur</t>
+  </si>
+  <si>
+    <t>Set up as per document</t>
+  </si>
+  <si>
+    <t>Set up the Use case 2 code "servicecore" zip file in hybris</t>
+  </si>
+  <si>
+    <t>The promotions notifications showing on IOS App - The welcome message is coming as heading for the promotions. We need to show the welcome messages separately</t>
+  </si>
+  <si>
+    <t>Send the geoLocation data of the user. And show the message and promotions that are returned as the json body of the response</t>
+  </si>
+  <si>
+    <t>URL : /greetCustomer
+POST
+Request Body
+{
+"latitude":"12.32",
+"longitude":"10.23",
+"customerId":"example@email.com"
+}
+Response Body
+Will update shortly</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Make the welcome message as a separate notification</t>
+  </si>
+  <si>
+    <t>related to the above point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test and fix the weather code. </t>
+  </si>
+  <si>
+    <t>Integrate the HTML for orders dashboard.</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -960,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1135,6 +1184,39 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1438,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3174,7 +3256,7 @@
         <v>42144</v>
       </c>
       <c r="E29" s="60">
-        <v>42144</v>
+        <v>42145</v>
       </c>
       <c r="F29" s="59" t="s">
         <v>41</v>
@@ -3194,7 +3276,7 @@
         <v>42144</v>
       </c>
       <c r="E30" s="57">
-        <v>42144</v>
+        <v>42145</v>
       </c>
       <c r="F30" s="54" t="s">
         <v>40</v>
@@ -3205,9 +3287,280 @@
       <c r="H30" s="54" t="s">
         <v>45</v>
       </c>
+    </row>
+    <row r="31" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="55"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="57">
+        <v>42149</v>
+      </c>
+      <c r="E31" s="57">
+        <v>42150</v>
+      </c>
+      <c r="F31" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="54"/>
+      <c r="D32" s="57">
+        <v>42150</v>
+      </c>
+      <c r="E32" s="57">
+        <v>42153</v>
+      </c>
+      <c r="F32" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="H32" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="59.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="71.42578125" style="62" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="63">
+        <v>0</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="63">
+        <v>0</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65">
+        <v>42149</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="63">
+        <v>1</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="63">
+        <v>1</v>
+      </c>
+      <c r="D3" s="65">
+        <v>42149</v>
+      </c>
+      <c r="E3" s="65">
+        <v>42150</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="44"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="63">
+        <v>2</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="64">
+        <v>1</v>
+      </c>
+      <c r="D4" s="65">
+        <v>42150</v>
+      </c>
+      <c r="E4" s="65">
+        <v>42151</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="44"/>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="63">
+        <v>3</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="64">
+        <v>1</v>
+      </c>
+      <c r="D5" s="65">
+        <v>42151</v>
+      </c>
+      <c r="E5" s="65">
+        <v>42152</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="66"/>
+      <c r="H5" s="44"/>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="63">
+        <v>4</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="64">
+        <v>1</v>
+      </c>
+      <c r="D6" s="65">
+        <v>42152</v>
+      </c>
+      <c r="E6" s="65">
+        <v>42153</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="66"/>
+      <c r="H6" s="44"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="63">
+        <v>5</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="64">
+        <v>2</v>
+      </c>
+      <c r="D7" s="65">
+        <v>42156</v>
+      </c>
+      <c r="E7" s="65">
+        <v>42157</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="66"/>
+      <c r="H7" s="44"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="63">
+        <v>6</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="65">
+        <v>42157</v>
+      </c>
+      <c r="E8" s="65">
+        <v>42157</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="44"/>
+    </row>
+    <row r="9" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A9" s="63">
+        <v>7</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="64">
+        <v>2</v>
+      </c>
+      <c r="D9" s="65">
+        <v>42158</v>
+      </c>
+      <c r="E9" s="65">
+        <v>42159</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated number of hours for IOS tasks
</commit_message>
<xml_diff>
--- a/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
+++ b/docs/DevTask_UseCase2_HealthProductsPromotion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Addtnl Tasks" sheetId="4" r:id="rId3"/>
     <sheet name="IOS Dev" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="138">
   <si>
     <t>S.No</t>
   </si>
@@ -761,6 +761,9 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>Effort(hours)</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1189,9 +1192,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2648,7 +2648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+    <sheetView topLeftCell="C28" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -3334,43 +3334,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="59.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="59.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="71.42578125" style="62" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="69" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="69" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3378,20 +3378,18 @@
       <c r="A2" s="63">
         <v>0</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="63">
-        <v>0</v>
-      </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65">
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64">
         <v>42149</v>
       </c>
       <c r="F2" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="67" t="s">
         <v>126</v>
       </c>
       <c r="H2" s="44" t="s">
@@ -3402,22 +3400,22 @@
       <c r="A3" s="63">
         <v>1</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="63">
-        <v>1</v>
-      </c>
-      <c r="D3" s="65">
+      <c r="C3" s="71">
+        <v>9</v>
+      </c>
+      <c r="D3" s="64">
         <v>42149</v>
       </c>
-      <c r="E3" s="65">
+      <c r="E3" s="64">
         <v>42150</v>
       </c>
       <c r="F3" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="67" t="s">
         <v>126</v>
       </c>
       <c r="H3" s="44"/>
@@ -3429,19 +3427,19 @@
       <c r="B4" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="64">
-        <v>1</v>
-      </c>
-      <c r="D4" s="65">
+      <c r="C4" s="45">
+        <v>8</v>
+      </c>
+      <c r="D4" s="64">
         <v>42150</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="64">
         <v>42151</v>
       </c>
       <c r="F4" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="65" t="s">
         <v>132</v>
       </c>
       <c r="H4" s="44"/>
@@ -3453,19 +3451,19 @@
       <c r="B5" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="64">
-        <v>1</v>
-      </c>
-      <c r="D5" s="65">
+      <c r="C5" s="45">
+        <v>10</v>
+      </c>
+      <c r="D5" s="64">
         <v>42151</v>
       </c>
-      <c r="E5" s="65">
+      <c r="E5" s="64">
         <v>42152</v>
       </c>
       <c r="F5" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="66"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="44"/>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3475,19 +3473,19 @@
       <c r="B6" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="64">
-        <v>1</v>
-      </c>
-      <c r="D6" s="65">
+      <c r="C6" s="45">
+        <v>9</v>
+      </c>
+      <c r="D6" s="64">
         <v>42152</v>
       </c>
-      <c r="E6" s="65">
+      <c r="E6" s="64">
         <v>42153</v>
       </c>
       <c r="F6" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="66"/>
+      <c r="G6" s="65"/>
       <c r="H6" s="44"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3497,19 +3495,19 @@
       <c r="B7" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="64">
-        <v>2</v>
-      </c>
-      <c r="D7" s="65">
+      <c r="C7" s="45">
+        <v>18</v>
+      </c>
+      <c r="D7" s="64">
         <v>42156</v>
       </c>
-      <c r="E7" s="65">
+      <c r="E7" s="64">
         <v>42157</v>
       </c>
       <c r="F7" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="G7" s="66"/>
+      <c r="G7" s="65"/>
       <c r="H7" s="44"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3519,19 +3517,19 @@
       <c r="B8" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="64">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="65">
+      <c r="C8" s="45">
+        <v>5</v>
+      </c>
+      <c r="D8" s="64">
         <v>42157</v>
       </c>
-      <c r="E8" s="65">
+      <c r="E8" s="64">
         <v>42157</v>
       </c>
       <c r="F8" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="G8" s="66" t="s">
+      <c r="G8" s="65" t="s">
         <v>133</v>
       </c>
       <c r="H8" s="44"/>
@@ -3540,22 +3538,22 @@
       <c r="A9" s="63">
         <v>7</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="64">
-        <v>2</v>
-      </c>
-      <c r="D9" s="65">
+      <c r="C9" s="66">
+        <v>25</v>
+      </c>
+      <c r="D9" s="64">
         <v>42158</v>
       </c>
-      <c r="E9" s="65">
+      <c r="E9" s="64">
         <v>42159</v>
       </c>
       <c r="F9" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="67" t="s">
         <v>130</v>
       </c>
       <c r="H9" s="44"/>

</xml_diff>